<commit_message>
[Fixed] Subida/Bajada Excel Materias Primas
</commit_message>
<xml_diff>
--- a/formatos/formato-materia-prima.xlsx
+++ b/formatos/formato-materia-prima.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\tezliksoftware\htdocs\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Tezlik\htdocs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DE420E-24CC-4B28-90EE-A993D505EEBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3EDD69-7FB4-4D45-AA59-2E3EEC632106}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materiales" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Unidad</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Materia Prima</t>
+  </si>
+  <si>
+    <t>Referencia</t>
   </si>
 </sst>
 </file>
@@ -484,20 +487,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11" style="4"/>
+    <col min="1" max="1" width="9.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="11" style="6"/>
     <col min="4" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -562,8 +568,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>